<commit_message>
Update Release-Notes.xlsx - Folder inventory updated on Sun Jun 15 01:07:43 UTC 2025
</commit_message>
<xml_diff>
--- a/Release-Notes.xlsx
+++ b/Release-Notes.xlsx
@@ -2288,7 +2288,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-06-12 10:29:52 UTC</t>
+          <t>2025-06-15 01:07:43 UTC</t>
         </is>
       </c>
     </row>
@@ -2310,7 +2310,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
     </row>

</xml_diff>